<commit_message>
permirsimi i kateve emri i gjeodetit dhe data
</commit_message>
<xml_diff>
--- a/3-Katet/regjistri/29-Koordinatat-e-kateve-2602-0-Albnori.xlsx
+++ b/3-Katet/regjistri/29-Koordinatat-e-kateve-2602-0-Albnori.xlsx
@@ -69,9 +69,6 @@
 </t>
   </si>
   <si>
-    <t>Sead Prushi</t>
-  </si>
-  <si>
     <t>Sqarim</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   <si>
     <t>Gjithsej</t>
   </si>
+  <si>
+    <t>Liridon Sejdiu</t>
+  </si>
 </sst>
 </file>
 
@@ -716,133 +716,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -853,6 +730,112 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -871,10 +854,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1834,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A103" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A70" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="S82" sqref="S82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,115 +1851,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1970,28 +1970,28 @@
       <c r="I12" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="61" t="s">
+      <c r="E14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="61" t="s">
+      <c r="F14" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="61" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="61" t="s">
+      <c r="H14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="27" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2009,15 +2009,15 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="65">
+      <c r="I15" s="79">
         <v>125.2</v>
       </c>
     </row>
@@ -2035,11 +2035,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="80"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
@@ -2055,11 +2055,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="80"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
@@ -2075,11 +2075,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="80"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
@@ -2095,11 +2095,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="80"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
@@ -2115,11 +2115,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="80"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="16">
@@ -2135,11 +2135,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="80"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="16">
@@ -2155,11 +2155,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="16">
@@ -2175,11 +2175,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="80"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
@@ -2195,11 +2195,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
@@ -2215,11 +2215,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="80"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
@@ -2235,11 +2235,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="67"/>
+        <v>24</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="81"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="16">
@@ -2255,13 +2255,13 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="63" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="68">
+        <v>25</v>
+      </c>
+      <c r="G27" s="49"/>
+      <c r="H27" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="77">
         <v>7.32</v>
       </c>
     </row>
@@ -2279,11 +2279,11 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="69"/>
+        <v>25</v>
+      </c>
+      <c r="G28" s="49"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="78"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="16">
@@ -2299,13 +2299,13 @@
         <v>620.11199999999997</v>
       </c>
       <c r="F29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="H29" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="70">
+      <c r="I29" s="29">
         <f>I15+I16+I17+I18+I19+I20+I21+I22+I23+I24+I25+I26+I27+I28</f>
         <v>132.52000000000001</v>
       </c>
@@ -2314,11 +2314,11 @@
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="73"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
@@ -2331,16 +2331,16 @@
         <v>1</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>7</v>
@@ -2360,15 +2360,15 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="H32" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="27">
+      <c r="I32" s="48">
         <v>141.58000000000001</v>
       </c>
     </row>
@@ -2386,11 +2386,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="17">
@@ -2406,11 +2406,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="17">
@@ -2426,11 +2426,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="17">
@@ -2446,11 +2446,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
@@ -2466,11 +2466,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="17">
@@ -2486,11 +2486,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="17">
@@ -2506,11 +2506,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="17">
@@ -2526,11 +2526,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="17">
@@ -2546,11 +2546,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="17">
@@ -2566,11 +2566,11 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
     </row>
     <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="18">
@@ -2586,13 +2586,13 @@
         <v>623.17399999999998</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="29">
+      <c r="G43" s="68"/>
+      <c r="H43" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="68">
         <f>SUM(I32:I40)</f>
         <v>141.58000000000001</v>
       </c>
@@ -2616,16 +2616,16 @@
         <v>1</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G45" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I45" s="12" t="s">
         <v>7</v>
@@ -2645,15 +2645,15 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G46" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="77">
+      <c r="H46" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="72">
         <v>128.09</v>
       </c>
     </row>
@@ -2671,11 +2671,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" s="59"/>
-      <c r="H47" s="75"/>
-      <c r="I47" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G47" s="46"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="73"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="17">
@@ -2691,11 +2691,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" s="59"/>
-      <c r="H48" s="75"/>
-      <c r="I48" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G48" s="46"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="73"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="17">
@@ -2711,11 +2711,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" s="59"/>
-      <c r="H49" s="75"/>
-      <c r="I49" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G49" s="46"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="73"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="17">
@@ -2731,11 +2731,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G50" s="59"/>
-      <c r="H50" s="75"/>
-      <c r="I50" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G50" s="46"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="73"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="17">
@@ -2751,11 +2751,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G51" s="59"/>
-      <c r="H51" s="75"/>
-      <c r="I51" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G51" s="46"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="73"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="17">
@@ -2771,11 +2771,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G52" s="59"/>
-      <c r="H52" s="75"/>
-      <c r="I52" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G52" s="46"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="73"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="17">
@@ -2791,11 +2791,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G53" s="59"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="78"/>
+        <v>27</v>
+      </c>
+      <c r="G53" s="46"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="73"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="17">
@@ -2811,11 +2811,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G54" s="59"/>
-      <c r="H54" s="75"/>
-      <c r="I54" s="78"/>
+        <v>19</v>
+      </c>
+      <c r="G54" s="46"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="73"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="17">
@@ -2831,11 +2831,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" s="59"/>
-      <c r="H55" s="75"/>
-      <c r="I55" s="78"/>
+        <v>19</v>
+      </c>
+      <c r="G55" s="46"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="73"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="17">
@@ -2851,11 +2851,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G56" s="59"/>
-      <c r="H56" s="75"/>
-      <c r="I56" s="78"/>
+        <v>19</v>
+      </c>
+      <c r="G56" s="46"/>
+      <c r="H56" s="70"/>
+      <c r="I56" s="73"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="17">
@@ -2871,11 +2871,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" s="59"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="78"/>
+        <v>19</v>
+      </c>
+      <c r="G57" s="46"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="73"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="17">
@@ -2891,11 +2891,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G58" s="59"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="78"/>
+        <v>19</v>
+      </c>
+      <c r="G58" s="46"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="73"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="17">
@@ -2911,11 +2911,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59" s="59"/>
-      <c r="H59" s="76"/>
-      <c r="I59" s="79"/>
+        <v>19</v>
+      </c>
+      <c r="G59" s="46"/>
+      <c r="H59" s="71"/>
+      <c r="I59" s="74"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="17">
@@ -2931,11 +2931,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G60" s="59"/>
+        <v>28</v>
+      </c>
+      <c r="G60" s="46"/>
       <c r="H60" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I60" s="26">
         <v>3.74</v>
@@ -2955,9 +2955,9 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G61" s="59"/>
+        <v>28</v>
+      </c>
+      <c r="G61" s="46"/>
       <c r="H61" s="25"/>
       <c r="I61" s="26"/>
     </row>
@@ -2975,11 +2975,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G62" s="59"/>
+        <v>28</v>
+      </c>
+      <c r="G62" s="46"/>
       <c r="H62" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I62" s="26">
         <v>5.88</v>
@@ -2999,9 +2999,9 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G63" s="59"/>
+        <v>28</v>
+      </c>
+      <c r="G63" s="46"/>
       <c r="H63" s="25"/>
       <c r="I63" s="26"/>
     </row>
@@ -3019,11 +3019,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G64" s="59"/>
+        <v>28</v>
+      </c>
+      <c r="G64" s="46"/>
       <c r="H64" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I64" s="26">
         <v>3.9</v>
@@ -3043,11 +3043,11 @@
         <v>626.09400000000005</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G65" s="60"/>
+        <v>28</v>
+      </c>
+      <c r="G65" s="47"/>
       <c r="H65" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I65" s="22">
         <v>141.61000000000001</v>
@@ -3164,145 +3164,145 @@
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="51"/>
-      <c r="G79" s="52"/>
-      <c r="H79" s="46" t="s">
+      <c r="E79" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F79" s="52"/>
+      <c r="G79" s="53"/>
+      <c r="H79" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I79" s="47"/>
-      <c r="J79" s="41"/>
-      <c r="K79" s="42"/>
+      <c r="I79" s="55"/>
+      <c r="J79" s="58"/>
+      <c r="K79" s="59"/>
     </row>
     <row r="80" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B80" s="54"/>
-      <c r="C80" s="54"/>
-      <c r="D80" s="55"/>
-      <c r="E80" s="56">
-        <v>152</v>
-      </c>
-      <c r="F80" s="57"/>
-      <c r="G80" s="58"/>
-      <c r="H80" s="48"/>
-      <c r="I80" s="49"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="44"/>
+      <c r="B80" s="63"/>
+      <c r="C80" s="63"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="65">
+        <v>140</v>
+      </c>
+      <c r="F80" s="66"/>
+      <c r="G80" s="67"/>
+      <c r="H80" s="56"/>
+      <c r="I80" s="57"/>
+      <c r="J80" s="60"/>
+      <c r="K80" s="61"/>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="30"/>
-      <c r="I81" s="30"/>
-      <c r="J81" s="30"/>
-      <c r="K81" s="30"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="35"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="35"/>
+      <c r="H81" s="35"/>
+      <c r="I81" s="35"/>
+      <c r="J81" s="35"/>
+      <c r="K81" s="35"/>
     </row>
     <row r="82" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="30"/>
-      <c r="I82" s="30"/>
-      <c r="J82" s="30"/>
-      <c r="K82" s="30"/>
+      <c r="A82" s="35"/>
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="35"/>
+      <c r="J82" s="35"/>
+      <c r="K82" s="35"/>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A83" s="45" t="s">
+      <c r="A83" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="45"/>
-      <c r="C83" s="45"/>
-      <c r="D83" s="45"/>
-      <c r="E83" s="45"/>
-      <c r="F83" s="45"/>
-      <c r="G83" s="45"/>
-      <c r="H83" s="45"/>
-      <c r="I83" s="45"/>
-      <c r="J83" s="45"/>
-      <c r="K83" s="45"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="36"/>
+      <c r="I83" s="36"/>
+      <c r="J83" s="36"/>
+      <c r="K83" s="36"/>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A84" s="45"/>
-      <c r="B84" s="45"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="45"/>
-      <c r="F84" s="45"/>
-      <c r="G84" s="45"/>
-      <c r="H84" s="45"/>
-      <c r="I84" s="45"/>
-      <c r="J84" s="45"/>
-      <c r="K84" s="45"/>
+      <c r="A84" s="36"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="36"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="36"/>
+      <c r="I84" s="36"/>
+      <c r="J84" s="36"/>
+      <c r="K84" s="36"/>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="45"/>
-      <c r="B85" s="45"/>
-      <c r="C85" s="45"/>
-      <c r="D85" s="45"/>
-      <c r="E85" s="45"/>
-      <c r="F85" s="45"/>
-      <c r="G85" s="45"/>
-      <c r="H85" s="45"/>
-      <c r="I85" s="45"/>
-      <c r="J85" s="45"/>
-      <c r="K85" s="45"/>
+      <c r="A85" s="36"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="36"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="36"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="36"/>
+      <c r="I85" s="36"/>
+      <c r="J85" s="36"/>
+      <c r="K85" s="36"/>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="45"/>
-      <c r="B86" s="45"/>
-      <c r="C86" s="45"/>
-      <c r="D86" s="45"/>
-      <c r="E86" s="45"/>
-      <c r="F86" s="45"/>
-      <c r="G86" s="45"/>
-      <c r="H86" s="45"/>
-      <c r="I86" s="45"/>
-      <c r="J86" s="45"/>
-      <c r="K86" s="45"/>
+      <c r="A86" s="36"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="36"/>
+      <c r="I86" s="36"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
     </row>
     <row r="87" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C88" s="31"/>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="32"/>
-      <c r="I88" s="32"/>
-      <c r="J88" s="33"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="39"/>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C89" s="34"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="35"/>
-      <c r="I89" s="35"/>
-      <c r="J89" s="36"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="41"/>
+      <c r="E89" s="41"/>
+      <c r="F89" s="41"/>
+      <c r="G89" s="41"/>
+      <c r="H89" s="41"/>
+      <c r="I89" s="41"/>
+      <c r="J89" s="42"/>
     </row>
     <row r="90" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C90" s="37"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="38"/>
-      <c r="J90" s="39"/>
+      <c r="C90" s="43"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+      <c r="I90" s="44"/>
+      <c r="J90" s="45"/>
     </row>
     <row r="91" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="6"/>
@@ -3323,16 +3323,16 @@
         <v>1</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H92" s="11" t="s">
         <v>6</v>
       </c>
       <c r="I92" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J92" s="12" t="s">
         <v>7</v>
@@ -3352,15 +3352,15 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="I93" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="J93" s="27">
+        <v>29</v>
+      </c>
+      <c r="H93" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="I93" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="J93" s="48">
         <v>101.28</v>
       </c>
     </row>
@@ -3378,11 +3378,11 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H94" s="59"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
+        <v>29</v>
+      </c>
+      <c r="H94" s="46"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="49"/>
       <c r="N94" s="24"/>
       <c r="O94" s="24"/>
       <c r="P94" s="24"/>
@@ -3407,19 +3407,19 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H95" s="59"/>
-      <c r="I95" s="28"/>
-      <c r="J95" s="28"/>
+        <v>29</v>
+      </c>
+      <c r="H95" s="46"/>
+      <c r="I95" s="49"/>
+      <c r="J95" s="49"/>
       <c r="N95" s="23"/>
       <c r="O95" s="23"/>
       <c r="P95" s="6"/>
       <c r="Q95" s="7"/>
       <c r="R95" s="7"/>
-      <c r="S95" s="71"/>
-      <c r="T95" s="80"/>
-      <c r="U95" s="80"/>
+      <c r="S95" s="30"/>
+      <c r="T95" s="33"/>
+      <c r="U95" s="33"/>
       <c r="V95" s="23"/>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
@@ -3436,19 +3436,19 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H96" s="59"/>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
+        <v>29</v>
+      </c>
+      <c r="H96" s="46"/>
+      <c r="I96" s="49"/>
+      <c r="J96" s="49"/>
       <c r="N96" s="23"/>
       <c r="O96" s="23"/>
       <c r="P96" s="6"/>
       <c r="Q96" s="7"/>
       <c r="R96" s="7"/>
-      <c r="S96" s="71"/>
-      <c r="T96" s="80"/>
-      <c r="U96" s="80"/>
+      <c r="S96" s="30"/>
+      <c r="T96" s="33"/>
+      <c r="U96" s="33"/>
       <c r="V96" s="23"/>
     </row>
     <row r="97" spans="3:22" x14ac:dyDescent="0.25">
@@ -3465,19 +3465,19 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H97" s="59"/>
-      <c r="I97" s="40"/>
-      <c r="J97" s="40"/>
+        <v>29</v>
+      </c>
+      <c r="H97" s="46"/>
+      <c r="I97" s="50"/>
+      <c r="J97" s="50"/>
       <c r="N97" s="23"/>
       <c r="O97" s="23"/>
       <c r="P97" s="6"/>
       <c r="Q97" s="7"/>
       <c r="R97" s="7"/>
-      <c r="S97" s="71"/>
-      <c r="T97" s="80"/>
-      <c r="U97" s="80"/>
+      <c r="S97" s="30"/>
+      <c r="T97" s="33"/>
+      <c r="U97" s="33"/>
       <c r="V97" s="23"/>
     </row>
     <row r="98" spans="3:22" x14ac:dyDescent="0.25">
@@ -3494,13 +3494,13 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H98" s="59"/>
-      <c r="I98" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="J98" s="27">
+        <v>30</v>
+      </c>
+      <c r="H98" s="46"/>
+      <c r="I98" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="J98" s="48">
         <v>40.29</v>
       </c>
       <c r="N98" s="23"/>
@@ -3508,9 +3508,9 @@
       <c r="P98" s="6"/>
       <c r="Q98" s="7"/>
       <c r="R98" s="7"/>
-      <c r="S98" s="71"/>
-      <c r="T98" s="80"/>
-      <c r="U98" s="80"/>
+      <c r="S98" s="30"/>
+      <c r="T98" s="33"/>
+      <c r="U98" s="33"/>
       <c r="V98" s="23"/>
     </row>
     <row r="99" spans="3:22" x14ac:dyDescent="0.25">
@@ -3527,19 +3527,19 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H99" s="59"/>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
+        <v>30</v>
+      </c>
+      <c r="H99" s="46"/>
+      <c r="I99" s="49"/>
+      <c r="J99" s="49"/>
       <c r="N99" s="23"/>
       <c r="O99" s="23"/>
       <c r="P99" s="6"/>
       <c r="Q99" s="7"/>
       <c r="R99" s="7"/>
-      <c r="S99" s="71"/>
-      <c r="T99" s="80"/>
-      <c r="U99" s="80"/>
+      <c r="S99" s="30"/>
+      <c r="T99" s="33"/>
+      <c r="U99" s="33"/>
       <c r="V99" s="23"/>
     </row>
     <row r="100" spans="3:22" x14ac:dyDescent="0.25">
@@ -3556,19 +3556,19 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H100" s="59"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="H100" s="46"/>
+      <c r="I100" s="49"/>
+      <c r="J100" s="49"/>
       <c r="N100" s="23"/>
       <c r="O100" s="23"/>
       <c r="P100" s="6"/>
       <c r="Q100" s="7"/>
       <c r="R100" s="7"/>
-      <c r="S100" s="71"/>
-      <c r="T100" s="80"/>
-      <c r="U100" s="80"/>
+      <c r="S100" s="30"/>
+      <c r="T100" s="33"/>
+      <c r="U100" s="33"/>
       <c r="V100" s="23"/>
     </row>
     <row r="101" spans="3:22" x14ac:dyDescent="0.25">
@@ -3585,17 +3585,17 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H101" s="59"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="H101" s="46"/>
+      <c r="I101" s="49"/>
+      <c r="J101" s="49"/>
       <c r="N101" s="23"/>
       <c r="O101" s="23"/>
       <c r="P101" s="6"/>
       <c r="Q101" s="7"/>
       <c r="R101" s="7"/>
-      <c r="S101" s="71"/>
+      <c r="S101" s="30"/>
       <c r="T101" s="9"/>
       <c r="U101" s="9"/>
       <c r="V101" s="23"/>
@@ -3614,17 +3614,17 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H102" s="59"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="H102" s="46"/>
+      <c r="I102" s="49"/>
+      <c r="J102" s="49"/>
       <c r="N102" s="23"/>
       <c r="O102" s="23"/>
       <c r="P102" s="6"/>
       <c r="Q102" s="7"/>
       <c r="R102" s="7"/>
-      <c r="S102" s="71"/>
+      <c r="S102" s="30"/>
       <c r="T102" s="24"/>
       <c r="U102" s="24"/>
       <c r="V102" s="23"/>
@@ -3643,11 +3643,11 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H103" s="59"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="H103" s="46"/>
+      <c r="I103" s="49"/>
+      <c r="J103" s="49"/>
       <c r="P103" s="6"/>
       <c r="Q103" s="7"/>
       <c r="R103" s="7"/>
@@ -3669,11 +3669,11 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H104" s="59"/>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="H104" s="46"/>
+      <c r="I104" s="49"/>
+      <c r="J104" s="49"/>
       <c r="N104" s="23"/>
       <c r="O104" s="23"/>
       <c r="P104" s="6"/>
@@ -3697,11 +3697,11 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H105" s="59"/>
-      <c r="I105" s="40"/>
-      <c r="J105" s="40"/>
+        <v>31</v>
+      </c>
+      <c r="H105" s="46"/>
+      <c r="I105" s="50"/>
+      <c r="J105" s="50"/>
     </row>
     <row r="106" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C106" s="18">
@@ -3717,13 +3717,13 @@
         <v>629.29999999999995</v>
       </c>
       <c r="G106" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H106" s="47"/>
+      <c r="I106" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="H106" s="60"/>
-      <c r="I106" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J106" s="81">
+      <c r="J106" s="34">
         <f>SUM(J93:J105)</f>
         <v>141.57</v>
       </c>
@@ -3852,34 +3852,34 @@
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
-      <c r="E129" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F129" s="51"/>
-      <c r="G129" s="52"/>
-      <c r="H129" s="46" t="s">
+      <c r="E129" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F129" s="52"/>
+      <c r="G129" s="53"/>
+      <c r="H129" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I129" s="47"/>
-      <c r="J129" s="41"/>
-      <c r="K129" s="42"/>
+      <c r="I129" s="55"/>
+      <c r="J129" s="58"/>
+      <c r="K129" s="59"/>
     </row>
     <row r="130" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="53" t="s">
+      <c r="A130" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B130" s="54"/>
-      <c r="C130" s="54"/>
-      <c r="D130" s="55"/>
-      <c r="E130" s="56">
-        <v>152</v>
-      </c>
-      <c r="F130" s="57"/>
-      <c r="G130" s="58"/>
-      <c r="H130" s="48"/>
-      <c r="I130" s="49"/>
-      <c r="J130" s="43"/>
-      <c r="K130" s="44"/>
+      <c r="B130" s="63"/>
+      <c r="C130" s="63"/>
+      <c r="D130" s="64"/>
+      <c r="E130" s="65">
+        <v>140</v>
+      </c>
+      <c r="F130" s="66"/>
+      <c r="G130" s="67"/>
+      <c r="H130" s="56"/>
+      <c r="I130" s="57"/>
+      <c r="J130" s="60"/>
+      <c r="K130" s="61"/>
     </row>
     <row r="131" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K131" s="1"/>
@@ -3892,6 +3892,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="C8:J10"/>
+    <mergeCell ref="J129:K130"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="H129:I130"/>
+    <mergeCell ref="E129:G129"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="E130:G130"/>
+    <mergeCell ref="G46:G65"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="H15:H26"/>
+    <mergeCell ref="I15:I26"/>
+    <mergeCell ref="G15:G29"/>
+    <mergeCell ref="G32:G43"/>
+    <mergeCell ref="H32:H43"/>
+    <mergeCell ref="I32:I43"/>
+    <mergeCell ref="H46:H59"/>
+    <mergeCell ref="I46:I59"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="H79:I80"/>
+    <mergeCell ref="J79:K80"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="E80:G80"/>
     <mergeCell ref="A81:K82"/>
     <mergeCell ref="A83:K86"/>
     <mergeCell ref="C88:J90"/>
@@ -3900,30 +3924,6 @@
     <mergeCell ref="J93:J97"/>
     <mergeCell ref="I98:I105"/>
     <mergeCell ref="J98:J105"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="H79:I80"/>
-    <mergeCell ref="J79:K80"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="G32:G43"/>
-    <mergeCell ref="H32:H43"/>
-    <mergeCell ref="I32:I43"/>
-    <mergeCell ref="H46:H59"/>
-    <mergeCell ref="I46:I59"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="H15:H26"/>
-    <mergeCell ref="I15:I26"/>
-    <mergeCell ref="G15:G29"/>
-    <mergeCell ref="J129:K130"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H129:I130"/>
-    <mergeCell ref="E129:G129"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="E130:G130"/>
-    <mergeCell ref="G46:G65"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="C8:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>